<commit_message>
Minor changes in results
</commit_message>
<xml_diff>
--- a/Testing Results/Results.xlsx
+++ b/Testing Results/Results.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ERDT\Desktop\FB Stories Folder\Testing results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robee Khyra Te\Documents\GitHub\storybook\Testing Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8268"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23010" windowHeight="8265"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" calcMode="manual"/>
+  <calcPr calcId="171027" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -273,8 +273,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -313,6 +313,13 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -465,7 +472,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -483,25 +490,54 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="2" fontId="5" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="5" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="5" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="5" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="5" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="6" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="6" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="6" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="6" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -778,17 +814,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="M38" sqref="M38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.109375" customWidth="1"/>
-    <col min="14" max="14" width="8.88671875" style="12"/>
+    <col min="1" max="1" width="48.140625" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -826,24 +862,24 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-    </row>
-    <row r="3" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+    </row>
+    <row r="3" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -883,12 +919,12 @@
       <c r="M3">
         <v>2</v>
       </c>
-      <c r="N3" s="12">
-        <f>AVERAGE($B3:$M3)</f>
+      <c r="N3" s="14">
+        <f t="shared" ref="N3:N11" si="0">AVERAGE($B3:$M3)</f>
         <v>2.5</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -928,12 +964,12 @@
       <c r="M4">
         <v>3</v>
       </c>
-      <c r="N4" s="12">
-        <f>AVERAGE($B4:$M4)</f>
+      <c r="N4" s="7">
+        <f t="shared" si="0"/>
         <v>3.1666666666666665</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -973,12 +1009,12 @@
       <c r="M5">
         <v>3</v>
       </c>
-      <c r="N5" s="12">
-        <f>AVERAGE($B5:$M5)</f>
+      <c r="N5" s="7">
+        <f t="shared" si="0"/>
         <v>3.1666666666666665</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -1018,12 +1054,12 @@
       <c r="M6">
         <v>3</v>
       </c>
-      <c r="N6" s="12">
-        <f>AVERAGE($B6:$M6)</f>
+      <c r="N6" s="14">
+        <f t="shared" si="0"/>
         <v>3.5833333333333335</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="29.4" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -1063,12 +1099,12 @@
       <c r="M7">
         <v>2</v>
       </c>
-      <c r="N7" s="12">
-        <f>AVERAGE($B7:$M7)</f>
+      <c r="N7" s="7">
+        <f t="shared" si="0"/>
         <v>2.9166666666666665</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="43.8" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:14" ht="45.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -1108,12 +1144,12 @@
       <c r="M8">
         <v>2</v>
       </c>
-      <c r="N8" s="12">
-        <f>AVERAGE($B8:$M8)</f>
+      <c r="N8" s="7">
+        <f t="shared" si="0"/>
         <v>2.5833333333333335</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -1153,12 +1189,12 @@
       <c r="M9">
         <v>3</v>
       </c>
-      <c r="N9" s="12">
-        <f>AVERAGE($B9:$M9)</f>
+      <c r="N9" s="7">
+        <f t="shared" si="0"/>
         <v>3.1666666666666665</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -1198,12 +1234,12 @@
       <c r="M10">
         <v>4</v>
       </c>
-      <c r="N10" s="12">
-        <f>AVERAGE($B10:$M10)</f>
+      <c r="N10" s="7">
+        <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="29.4" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -1243,29 +1279,29 @@
       <c r="M11">
         <v>2</v>
       </c>
-      <c r="N11" s="12">
-        <f>AVERAGE($B11:$M11)</f>
+      <c r="N11" s="7">
+        <f t="shared" si="0"/>
         <v>2.8333333333333335</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="8" t="s">
+    <row r="13" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
-    </row>
-    <row r="14" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+    </row>
+    <row r="14" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1305,129 +1341,129 @@
       <c r="M14">
         <v>4</v>
       </c>
-      <c r="N14" s="12">
+      <c r="N14" s="14">
         <f>AVERAGE($B14:$M14)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="10">
-        <v>2</v>
-      </c>
-      <c r="C15" s="9">
-        <v>4</v>
-      </c>
-      <c r="D15" s="9">
-        <v>4</v>
-      </c>
-      <c r="E15" s="16">
-        <v>4</v>
-      </c>
-      <c r="F15" s="16">
-        <v>4</v>
-      </c>
-      <c r="G15" s="16">
-        <v>2</v>
-      </c>
-      <c r="H15" s="16">
-        <v>4</v>
-      </c>
-      <c r="I15" s="16">
-        <v>3</v>
-      </c>
-      <c r="J15" s="9">
-        <v>4</v>
-      </c>
-      <c r="K15" s="16">
-        <v>4</v>
-      </c>
-      <c r="L15" s="16">
-        <v>4</v>
-      </c>
-      <c r="M15" s="11">
-        <v>4</v>
-      </c>
-      <c r="N15" s="13">
+      <c r="B15" s="11">
+        <v>2</v>
+      </c>
+      <c r="C15" s="10">
+        <v>4</v>
+      </c>
+      <c r="D15" s="10">
+        <v>4</v>
+      </c>
+      <c r="E15" s="8">
+        <v>4</v>
+      </c>
+      <c r="F15" s="8">
+        <v>4</v>
+      </c>
+      <c r="G15" s="8">
+        <v>2</v>
+      </c>
+      <c r="H15" s="8">
+        <v>4</v>
+      </c>
+      <c r="I15" s="8">
+        <v>3</v>
+      </c>
+      <c r="J15" s="10">
+        <v>4</v>
+      </c>
+      <c r="K15" s="8">
+        <v>4</v>
+      </c>
+      <c r="L15" s="8">
+        <v>4</v>
+      </c>
+      <c r="M15" s="9">
+        <v>4</v>
+      </c>
+      <c r="N15" s="15">
         <f>AVERAGE($B15:$M15)</f>
         <v>3.5833333333333335</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="16"/>
-      <c r="L16" s="16"/>
-      <c r="M16" s="11"/>
-      <c r="N16" s="14"/>
-    </row>
-    <row r="17" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="11"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="16"/>
+    </row>
+    <row r="17" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="16"/>
-      <c r="L17" s="16"/>
-      <c r="M17" s="11"/>
-      <c r="N17" s="14"/>
-    </row>
-    <row r="18" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B17" s="11"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="16"/>
+    </row>
+    <row r="18" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="10"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="16"/>
-      <c r="L18" s="16"/>
-      <c r="M18" s="11"/>
-      <c r="N18" s="14"/>
-    </row>
-    <row r="19" spans="1:14" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="11"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="16"/>
+    </row>
+    <row r="19" spans="1:14" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="16"/>
-      <c r="L19" s="16"/>
-      <c r="M19" s="11"/>
-      <c r="N19" s="15"/>
-    </row>
-    <row r="20" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B19" s="11"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="17"/>
+    </row>
+    <row r="20" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>34</v>
       </c>
@@ -1467,12 +1503,12 @@
       <c r="M20">
         <v>4</v>
       </c>
-      <c r="N20" s="12">
+      <c r="N20" s="14">
         <f>AVERAGE($B20:$M20)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="43.8" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:14" ht="60.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>18</v>
       </c>
@@ -1512,29 +1548,29 @@
       <c r="M21">
         <v>4</v>
       </c>
-      <c r="N21" s="12">
+      <c r="N21" s="7">
         <f>AVERAGE($B21:$M21)</f>
         <v>3.75</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="8" t="s">
+    <row r="23" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="8"/>
-      <c r="M23" s="8"/>
-    </row>
-    <row r="24" spans="1:14" ht="29.4" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+    </row>
+    <row r="24" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>20</v>
       </c>
@@ -1574,12 +1610,12 @@
       <c r="M24">
         <v>3</v>
       </c>
-      <c r="N24" s="12">
-        <f>AVERAGE($B24:$M24)</f>
+      <c r="N24" s="7">
+        <f t="shared" ref="N24:N32" si="1">AVERAGE($B24:$M24)</f>
         <v>3.4166666666666665</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="29.4" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>21</v>
       </c>
@@ -1619,12 +1655,12 @@
       <c r="M25">
         <v>3</v>
       </c>
-      <c r="N25" s="12">
-        <f>AVERAGE($B25:$M25)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" ht="43.8" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N25" s="14">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="45.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>22</v>
       </c>
@@ -1664,12 +1700,12 @@
       <c r="M26">
         <v>2</v>
       </c>
-      <c r="N26" s="12">
-        <f>AVERAGE($B26:$M26)</f>
+      <c r="N26" s="7">
+        <f t="shared" si="1"/>
         <v>3.0833333333333335</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="29.4" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:14" ht="45.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>23</v>
       </c>
@@ -1709,12 +1745,12 @@
       <c r="M27">
         <v>4</v>
       </c>
-      <c r="N27" s="12">
-        <f>AVERAGE($B27:$M27)</f>
+      <c r="N27" s="7">
+        <f t="shared" si="1"/>
         <v>3.5833333333333335</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>24</v>
       </c>
@@ -1754,12 +1790,12 @@
       <c r="M28">
         <v>3</v>
       </c>
-      <c r="N28" s="12">
-        <f>AVERAGE($B28:$M28)</f>
+      <c r="N28" s="7">
+        <f t="shared" si="1"/>
         <v>3.3333333333333335</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="29.4" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>25</v>
       </c>
@@ -1799,12 +1835,12 @@
       <c r="M29">
         <v>3</v>
       </c>
-      <c r="N29" s="12">
-        <f>AVERAGE($B29:$M29)</f>
+      <c r="N29" s="7">
+        <f t="shared" si="1"/>
         <v>3.5</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="43.8" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:14" ht="45.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>26</v>
       </c>
@@ -1844,12 +1880,12 @@
       <c r="M30">
         <v>3</v>
       </c>
-      <c r="N30" s="12">
-        <f>AVERAGE($B30:$M30)</f>
+      <c r="N30" s="7">
+        <f t="shared" si="1"/>
         <v>3.3333333333333335</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="29.4" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:14" ht="45.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>27</v>
       </c>
@@ -1889,12 +1925,12 @@
       <c r="M31">
         <v>3</v>
       </c>
-      <c r="N31" s="12">
-        <f>AVERAGE($B31:$M31)</f>
+      <c r="N31" s="14">
+        <f t="shared" si="1"/>
         <v>3.6666666666666665</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="29.4" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>28</v>
       </c>
@@ -1934,29 +1970,29 @@
       <c r="M32">
         <v>3</v>
       </c>
-      <c r="N32" s="12">
-        <f>AVERAGE($B32:$M32)</f>
+      <c r="N32" s="7">
+        <f t="shared" si="1"/>
         <v>3.5</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="8" t="s">
+    <row r="34" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8"/>
-      <c r="K34" s="8"/>
-      <c r="L34" s="8"/>
-      <c r="M34" s="8"/>
-    </row>
-    <row r="35" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="13"/>
+    </row>
+    <row r="35" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>30</v>
       </c>
@@ -1996,12 +2032,12 @@
       <c r="M35">
         <v>4</v>
       </c>
-      <c r="N35" s="12">
+      <c r="N35" s="7">
         <f>AVERAGE($B35:$M35)</f>
         <v>3.75</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="29.4" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>31</v>
       </c>
@@ -2041,12 +2077,12 @@
       <c r="M36">
         <v>4</v>
       </c>
-      <c r="N36" s="12">
+      <c r="N36" s="7">
         <f>AVERAGE($B36:$M36)</f>
         <v>3.75</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>32</v>
       </c>
@@ -2086,12 +2122,12 @@
       <c r="M37">
         <v>4</v>
       </c>
-      <c r="N37" s="12">
+      <c r="N37" s="7">
         <f>AVERAGE($B37:$M37)</f>
         <v>3.8333333333333335</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="29.4" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:14" ht="45.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>33</v>
       </c>
@@ -2131,63 +2167,73 @@
       <c r="M38">
         <v>4</v>
       </c>
-      <c r="N38" s="12">
+      <c r="N38" s="7">
         <f>AVERAGE($B38:$M38)</f>
         <v>3.8333333333333335</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B39">
         <f>AVERAGE(B$3:B$38)</f>
         <v>3.5769230769230771</v>
       </c>
       <c r="C39" s="6">
-        <f t="shared" ref="C39:M39" si="0">AVERAGE(C$3:C$38)</f>
+        <f t="shared" ref="C39:M39" si="2">AVERAGE(C$3:C$38)</f>
         <v>3.8076923076923075</v>
       </c>
       <c r="D39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.6538461538461537</v>
       </c>
       <c r="E39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.7692307692307692</v>
       </c>
       <c r="F39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.6153846153846154</v>
       </c>
       <c r="G39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.8846153846153846</v>
       </c>
       <c r="H39" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.2307692307692308</v>
       </c>
       <c r="I39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.8846153846153846</v>
       </c>
       <c r="J39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.6538461538461537</v>
       </c>
       <c r="K39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.2692307692307692</v>
       </c>
       <c r="L39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.2307692307692308</v>
       </c>
       <c r="M39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.1923076923076925</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A13:M13"/>
+    <mergeCell ref="A23:M23"/>
+    <mergeCell ref="A34:M34"/>
+    <mergeCell ref="B15:B19"/>
+    <mergeCell ref="C15:C19"/>
+    <mergeCell ref="N15:N19"/>
+    <mergeCell ref="D15:D19"/>
+    <mergeCell ref="E15:E19"/>
+    <mergeCell ref="F15:F19"/>
     <mergeCell ref="G15:G19"/>
     <mergeCell ref="H15:H19"/>
     <mergeCell ref="L15:L19"/>
@@ -2195,16 +2241,6 @@
     <mergeCell ref="J15:J19"/>
     <mergeCell ref="I15:I19"/>
     <mergeCell ref="K15:K19"/>
-    <mergeCell ref="B15:B19"/>
-    <mergeCell ref="C15:C19"/>
-    <mergeCell ref="N15:N19"/>
-    <mergeCell ref="D15:D19"/>
-    <mergeCell ref="E15:E19"/>
-    <mergeCell ref="F15:F19"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="A13:M13"/>
-    <mergeCell ref="A23:M23"/>
-    <mergeCell ref="A34:M34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>